<commit_message>
J-Teoria Estructuras V1 Prototypes
</commit_message>
<xml_diff>
--- a/Apuntes/LanguajePrototype/05-Introducción a Estructuras de datos/IntroEstructurasDeDatos.xlsx
+++ b/Apuntes/LanguajePrototype/05-Introducción a Estructuras de datos/IntroEstructurasDeDatos.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oscar Ardevol\Documents\VSC\Proyectos GitHub\Teoria\Apuntes\LanguajePrototype\05-Introducción a Estructuras de datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0874F604-BE2E-4440-9B46-D82D0D56EC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82323A11-F541-4179-83E6-52ED1DB07765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Estructuras" sheetId="1" r:id="rId1"/>
+    <sheet name="Estructurass" sheetId="2" r:id="rId1"/>
+    <sheet name="Matrices" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Separamos columnas y luego saltamos de fila. "Formato filas".</t>
   </si>
@@ -101,6 +102,42 @@
   </si>
   <si>
     <t>JSON</t>
+  </si>
+  <si>
+    <t>Listas</t>
+  </si>
+  <si>
+    <t>Tipos de estructuras</t>
+  </si>
+  <si>
+    <t>Equivalentes</t>
+  </si>
+  <si>
+    <t>Rangos</t>
+  </si>
+  <si>
+    <t>Tuplas</t>
+  </si>
+  <si>
+    <t>Matrices</t>
+  </si>
+  <si>
+    <t>Diccionarios</t>
+  </si>
+  <si>
+    <t>Tablas</t>
+  </si>
+  <si>
+    <t>Caracteriasticas</t>
+  </si>
+  <si>
+    <t>Sus valores son facilmente mutables</t>
+  </si>
+  <si>
+    <t>No se modifican a no ser que entres manualmente en la matriz original para cambiarlos</t>
+  </si>
+  <si>
+    <t>Tienen una estructura clave:valor. Columna : Fila/s.</t>
   </si>
 </sst>
 </file>
@@ -152,7 +189,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -434,11 +471,75 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE9957BD-2E97-45D7-9B92-C3C2C6F6D440}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="79.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>